<commit_message>
user management springboot project is updated
</commit_message>
<xml_diff>
--- a/project/Assignments/MRU_DS_Java_FSD_Assignment_2.xlsx
+++ b/project/Assignments/MRU_DS_Java_FSD_Assignment_2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ByteXL\MRU\Java_FSD\project\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E84A595-6587-4D15-B922-D7CC41309F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{420C0292-10AD-4DBC-B676-128863B64273}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Nimbus Evaluation Export" sheetId="1" r:id="rId1"/>
@@ -2263,7 +2262,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2840,51 +2839,52 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="23">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2934,6 +2934,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2942,7 +2962,48 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2957,7 +3018,48 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2972,7 +3074,6 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2987,37 +3088,6 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3032,25 +3102,9 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3132,23 +3186,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ABEB34E8-E56C-43A4-85AA-AB801A688D75}" name="Table1" displayName="Table1" ref="A9:I186" totalsRowShown="0" headerRowDxfId="0" dataDxfId="13">
-  <autoFilter ref="A9:I186" xr:uid="{ABEB34E8-E56C-43A4-85AA-AB801A688D75}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:I186">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:I186" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A9:I186"/>
+  <sortState ref="A10:I186">
     <sortCondition ref="A9:A186"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F1AAB9-C6CF-4A57-91A4-230449BEF881}" name="S.NO" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D2B48E2C-473F-4C20-B1D2-5AB158057F58}" name="NAME" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{55703D62-BA22-4005-9C2A-3204B87E2E92}" name="EMAIL" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{1EF93D95-3EB5-4ECC-BC5C-B5CB1F0AB4C7}" name="ROLL NO" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{1AB2F1F8-264B-48E7-BE46-84E25C723346}" name="DEPARTMENT" dataDxfId="10">
+    <tableColumn id="1" name="S.NO" dataDxfId="20"/>
+    <tableColumn id="2" name="NAME" dataDxfId="19"/>
+    <tableColumn id="3" name="EMAIL" dataDxfId="18"/>
+    <tableColumn id="4" name="ROLL NO" dataDxfId="17"/>
+    <tableColumn id="5" name="DEPARTMENT" dataDxfId="16">
       <calculatedColumnFormula>UPPER(Table1[[#This Row],[NAME]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FCFB51D3-EF03-46F2-88C5-FE9DF246BDD7}" name="BATCH" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{CE390982-D028-4EA6-8030-618743979E53}" name="NIMBUS URL" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{759625E8-D7CA-4717-86AD-0862EC023A3E}" name="GITHUB URL" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{90ED5D08-6A93-443A-92CC-6F8A351E338D}" name="DEMO URL" dataDxfId="14"/>
+    <tableColumn id="6" name="BATCH" dataDxfId="15"/>
+    <tableColumn id="7" name="NIMBUS URL" dataDxfId="14"/>
+    <tableColumn id="8" name="GITHUB URL" dataDxfId="13"/>
+    <tableColumn id="9" name="DEMO URL" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3450,24 +3504,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802AA8F2-91E1-4A87-A608-89D68FD3290F}">
-  <dimension ref="A1:I337"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="95.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="95.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="6" t="s">
         <v>715</v>
@@ -3482,7 +3538,7 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -3491,7 +3547,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>714</v>
@@ -3506,7 +3562,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3517,7 +3573,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -3532,7 +3588,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3543,7 +3599,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
@@ -3558,7 +3614,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -3587,7 +3643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -3616,7 +3672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -3645,7 +3701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -3674,7 +3730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -3703,7 +3759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -3732,7 +3788,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -3761,7 +3817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -3790,7 +3846,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -3819,7 +3875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -3848,7 +3904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -3877,7 +3933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -3906,7 +3962,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -3935,7 +3991,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -3964,7 +4020,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>14</v>
       </c>
@@ -3993,7 +4049,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>15</v>
       </c>
@@ -4022,7 +4078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>16</v>
       </c>
@@ -4051,7 +4107,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>17</v>
       </c>
@@ -4080,7 +4136,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>18</v>
       </c>
@@ -4109,7 +4165,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>19</v>
       </c>
@@ -4138,7 +4194,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>20</v>
       </c>
@@ -4167,7 +4223,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>21</v>
       </c>
@@ -4196,7 +4252,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>22</v>
       </c>
@@ -4225,7 +4281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>23</v>
       </c>
@@ -4254,7 +4310,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -4283,7 +4339,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>25</v>
       </c>
@@ -4312,7 +4368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>26</v>
       </c>
@@ -4341,7 +4397,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>27</v>
       </c>
@@ -4370,7 +4426,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>28</v>
       </c>
@@ -4399,7 +4455,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>29</v>
       </c>
@@ -4428,7 +4484,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>30</v>
       </c>
@@ -4457,7 +4513,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>31</v>
       </c>
@@ -4486,7 +4542,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>32</v>
       </c>
@@ -4515,7 +4571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>33</v>
       </c>
@@ -4544,7 +4600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>34</v>
       </c>
@@ -4573,7 +4629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>35</v>
       </c>
@@ -4602,7 +4658,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>36</v>
       </c>
@@ -4631,7 +4687,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>37</v>
       </c>
@@ -4660,7 +4716,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>38</v>
       </c>
@@ -4689,7 +4745,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>39</v>
       </c>
@@ -4718,7 +4774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>40</v>
       </c>
@@ -4747,7 +4803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>41</v>
       </c>
@@ -4776,7 +4832,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>42</v>
       </c>
@@ -4805,7 +4861,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>43</v>
       </c>
@@ -4834,7 +4890,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>44</v>
       </c>
@@ -4863,7 +4919,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>45</v>
       </c>
@@ -4892,7 +4948,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>46</v>
       </c>
@@ -4921,7 +4977,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>47</v>
       </c>
@@ -4950,7 +5006,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>48</v>
       </c>
@@ -4979,7 +5035,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>49</v>
       </c>
@@ -5008,7 +5064,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>50</v>
       </c>
@@ -5037,7 +5093,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>51</v>
       </c>
@@ -5066,7 +5122,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>52</v>
       </c>
@@ -5095,7 +5151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>53</v>
       </c>
@@ -5124,7 +5180,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>54</v>
       </c>
@@ -5153,7 +5209,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>55</v>
       </c>
@@ -5182,7 +5238,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>56</v>
       </c>
@@ -5211,7 +5267,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>57</v>
       </c>
@@ -5240,7 +5296,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>58</v>
       </c>
@@ -5269,7 +5325,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>59</v>
       </c>
@@ -5298,7 +5354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>60</v>
       </c>
@@ -5327,7 +5383,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>61</v>
       </c>
@@ -5356,7 +5412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>62</v>
       </c>
@@ -5385,7 +5441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>63</v>
       </c>
@@ -5414,7 +5470,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>64</v>
       </c>
@@ -5443,7 +5499,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>65</v>
       </c>
@@ -5472,7 +5528,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>66</v>
       </c>
@@ -5501,7 +5557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>67</v>
       </c>
@@ -5530,7 +5586,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>68</v>
       </c>
@@ -5559,7 +5615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>69</v>
       </c>
@@ -5588,7 +5644,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>70</v>
       </c>
@@ -5617,7 +5673,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>71</v>
       </c>
@@ -5646,7 +5702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>72</v>
       </c>
@@ -5675,7 +5731,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>73</v>
       </c>
@@ -5704,7 +5760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>74</v>
       </c>
@@ -5733,7 +5789,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>75</v>
       </c>
@@ -5762,7 +5818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>76</v>
       </c>
@@ -5791,7 +5847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>77</v>
       </c>
@@ -5820,7 +5876,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>78</v>
       </c>
@@ -5849,7 +5905,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>79</v>
       </c>
@@ -5878,7 +5934,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>80</v>
       </c>
@@ -5907,7 +5963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>81</v>
       </c>
@@ -5936,7 +5992,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>82</v>
       </c>
@@ -5965,7 +6021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>83</v>
       </c>
@@ -5994,7 +6050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>84</v>
       </c>
@@ -6023,7 +6079,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>85</v>
       </c>
@@ -6052,7 +6108,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>86</v>
       </c>
@@ -6081,7 +6137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>87</v>
       </c>
@@ -6110,7 +6166,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>88</v>
       </c>
@@ -6139,7 +6195,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>89</v>
       </c>
@@ -6168,7 +6224,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>90</v>
       </c>
@@ -6197,7 +6253,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>91</v>
       </c>
@@ -6226,7 +6282,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>92</v>
       </c>
@@ -6255,7 +6311,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>93</v>
       </c>
@@ -6284,7 +6340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>94</v>
       </c>
@@ -6313,7 +6369,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>95</v>
       </c>
@@ -6342,7 +6398,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>96</v>
       </c>
@@ -6371,7 +6427,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>97</v>
       </c>
@@ -6400,7 +6456,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>98</v>
       </c>
@@ -6429,7 +6485,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>99</v>
       </c>
@@ -6458,7 +6514,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>100</v>
       </c>
@@ -6487,7 +6543,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>101</v>
       </c>
@@ -6516,7 +6572,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>102</v>
       </c>
@@ -6545,7 +6601,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>103</v>
       </c>
@@ -6574,7 +6630,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>104</v>
       </c>
@@ -6603,7 +6659,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>105</v>
       </c>
@@ -6632,7 +6688,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>106</v>
       </c>
@@ -6661,7 +6717,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>107</v>
       </c>
@@ -6690,7 +6746,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>108</v>
       </c>
@@ -6719,7 +6775,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>109</v>
       </c>
@@ -6748,7 +6804,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>110</v>
       </c>
@@ -6777,7 +6833,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>111</v>
       </c>
@@ -6806,7 +6862,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>112</v>
       </c>
@@ -6835,7 +6891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>113</v>
       </c>
@@ -6864,7 +6920,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>114</v>
       </c>
@@ -6893,7 +6949,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>115</v>
       </c>
@@ -6922,7 +6978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>116</v>
       </c>
@@ -6951,7 +7007,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>117</v>
       </c>
@@ -6980,7 +7036,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>118</v>
       </c>
@@ -7009,7 +7065,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>119</v>
       </c>
@@ -7038,7 +7094,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>120</v>
       </c>
@@ -7067,7 +7123,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>121</v>
       </c>
@@ -7096,7 +7152,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>122</v>
       </c>
@@ -7125,7 +7181,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>123</v>
       </c>
@@ -7154,7 +7210,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>124</v>
       </c>
@@ -7183,7 +7239,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>125</v>
       </c>
@@ -7212,7 +7268,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>126</v>
       </c>
@@ -7241,7 +7297,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>127</v>
       </c>
@@ -7270,7 +7326,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>128</v>
       </c>
@@ -7299,7 +7355,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>129</v>
       </c>
@@ -7328,7 +7384,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>130</v>
       </c>
@@ -7357,7 +7413,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>131</v>
       </c>
@@ -7386,7 +7442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>132</v>
       </c>
@@ -7415,7 +7471,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>133</v>
       </c>
@@ -7444,7 +7500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>134</v>
       </c>
@@ -7473,7 +7529,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>135</v>
       </c>
@@ -7502,7 +7558,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>136</v>
       </c>
@@ -7531,7 +7587,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>137</v>
       </c>
@@ -7560,7 +7616,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>138</v>
       </c>
@@ -7589,7 +7645,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>139</v>
       </c>
@@ -7618,7 +7674,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>140</v>
       </c>
@@ -7647,7 +7703,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>141</v>
       </c>
@@ -7676,7 +7732,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>142</v>
       </c>
@@ -7705,7 +7761,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>143</v>
       </c>
@@ -7734,7 +7790,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>144</v>
       </c>
@@ -7763,7 +7819,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>145</v>
       </c>
@@ -7792,7 +7848,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>146</v>
       </c>
@@ -7821,7 +7877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>147</v>
       </c>
@@ -7850,7 +7906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>148</v>
       </c>
@@ -7879,7 +7935,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>149</v>
       </c>
@@ -7908,7 +7964,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>150</v>
       </c>
@@ -7937,7 +7993,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>151</v>
       </c>
@@ -7966,7 +8022,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>152</v>
       </c>
@@ -7995,7 +8051,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>153</v>
       </c>
@@ -8024,7 +8080,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>154</v>
       </c>
@@ -8053,7 +8109,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>155</v>
       </c>
@@ -8082,7 +8138,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>156</v>
       </c>
@@ -8111,7 +8167,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>157</v>
       </c>
@@ -8140,7 +8196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>158</v>
       </c>
@@ -8169,7 +8225,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>159</v>
       </c>
@@ -8198,7 +8254,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>160</v>
       </c>
@@ -8227,7 +8283,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>161</v>
       </c>
@@ -8256,7 +8312,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>162</v>
       </c>
@@ -8285,7 +8341,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>163</v>
       </c>
@@ -8314,7 +8370,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>164</v>
       </c>
@@ -8343,7 +8399,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>165</v>
       </c>
@@ -8372,7 +8428,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>166</v>
       </c>
@@ -8401,7 +8457,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>167</v>
       </c>
@@ -8430,7 +8486,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>168</v>
       </c>
@@ -8459,7 +8515,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>169</v>
       </c>
@@ -8488,7 +8544,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>170</v>
       </c>
@@ -8517,7 +8573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>171</v>
       </c>
@@ -8546,7 +8602,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>172</v>
       </c>
@@ -8575,7 +8631,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>173</v>
       </c>
@@ -8604,7 +8660,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>174</v>
       </c>
@@ -8633,7 +8689,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>175</v>
       </c>
@@ -8662,7 +8718,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>176</v>
       </c>
@@ -8691,7 +8747,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>177</v>
       </c>
@@ -8720,464 +8776,29 @@
         <v>388</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D188" s="7"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D189" s="7"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D190" s="7"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D191" s="7"/>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D192" s="7"/>
-    </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D193" s="7"/>
-    </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D194" s="7"/>
-    </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D195" s="7"/>
-    </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D196" s="7"/>
-    </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D197" s="7"/>
-    </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D198" s="7"/>
-    </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D199" s="7"/>
-    </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D200" s="7"/>
-    </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D201" s="7"/>
-    </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D202" s="7"/>
-    </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D203" s="7"/>
-    </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D204" s="7"/>
-    </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D205" s="7"/>
-    </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D206" s="7"/>
-    </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D207" s="7"/>
-    </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D208" s="7"/>
-    </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D209" s="7"/>
-    </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D210" s="7"/>
-    </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D211" s="7"/>
-    </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D212" s="7"/>
-    </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D213" s="7"/>
-    </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D214" s="7"/>
-    </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D215" s="7"/>
-    </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D216" s="7"/>
-    </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D217" s="7"/>
-    </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D218" s="7"/>
-    </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D219" s="7"/>
-    </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D220" s="7"/>
-    </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D221" s="7"/>
-    </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D222" s="7"/>
-    </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D223" s="7"/>
-    </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D224" s="7"/>
-    </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D225" s="7"/>
-    </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D226" s="7"/>
-    </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D227" s="7"/>
-    </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D228" s="7"/>
-    </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D229" s="7"/>
-    </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D230" s="7"/>
-    </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D231" s="7"/>
-    </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D232" s="7"/>
-    </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D233" s="7"/>
-    </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D234" s="7"/>
-    </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D235" s="7"/>
-    </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D236" s="7"/>
-    </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D237" s="7"/>
-    </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D238" s="7"/>
-    </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D239" s="7"/>
-    </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D240" s="7"/>
-    </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D241" s="7"/>
-    </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D242" s="7"/>
-    </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D243" s="7"/>
-    </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D244" s="7"/>
-    </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D245" s="7"/>
-    </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D246" s="7"/>
-    </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D247" s="7"/>
-    </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D248" s="7"/>
-    </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D249" s="7"/>
-    </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D250" s="7"/>
-    </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D251" s="7"/>
-    </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D252" s="7"/>
-    </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D253" s="7"/>
-    </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D254" s="7"/>
-    </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D255" s="7"/>
-    </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D256" s="7"/>
-    </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D257" s="7"/>
-    </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D258" s="7"/>
-    </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D259" s="7"/>
-    </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D260" s="7"/>
-    </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D261" s="7"/>
-    </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D262" s="7"/>
-    </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D263" s="7"/>
-    </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D264" s="7"/>
-    </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D265" s="7"/>
-    </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D266" s="7"/>
-    </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D267" s="7"/>
-    </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D268" s="7"/>
-    </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D269" s="7"/>
-    </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D270" s="7"/>
-    </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D271" s="7"/>
-    </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D272" s="7"/>
-    </row>
-    <row r="273" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D273" s="7"/>
-    </row>
-    <row r="274" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D274" s="7"/>
-    </row>
-    <row r="275" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D275" s="7"/>
-    </row>
-    <row r="276" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D276" s="7"/>
-    </row>
-    <row r="277" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D277" s="7"/>
-    </row>
-    <row r="278" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D278" s="7"/>
-    </row>
-    <row r="279" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D279" s="7"/>
-    </row>
-    <row r="280" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D280" s="7"/>
-    </row>
-    <row r="281" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D281" s="7"/>
-    </row>
-    <row r="282" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D282" s="7"/>
-    </row>
-    <row r="283" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D283" s="7"/>
-    </row>
-    <row r="284" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D284" s="7"/>
-    </row>
-    <row r="285" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D285" s="7"/>
-    </row>
-    <row r="286" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D286" s="7"/>
-    </row>
-    <row r="287" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D287" s="7"/>
-    </row>
-    <row r="288" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D288" s="7"/>
-    </row>
-    <row r="289" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D289" s="7"/>
-    </row>
-    <row r="290" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D290" s="7"/>
-    </row>
-    <row r="291" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D291" s="7"/>
-    </row>
-    <row r="292" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D292" s="7"/>
-    </row>
-    <row r="293" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D293" s="7"/>
-    </row>
-    <row r="294" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D294" s="7"/>
-    </row>
-    <row r="295" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D295" s="7"/>
-    </row>
-    <row r="296" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D296" s="7"/>
-    </row>
-    <row r="297" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D297" s="7"/>
-    </row>
-    <row r="298" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D298" s="7"/>
-    </row>
-    <row r="299" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D299" s="7"/>
-    </row>
-    <row r="300" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D300" s="7"/>
-    </row>
-    <row r="301" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D301" s="7"/>
-    </row>
-    <row r="302" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D302" s="7"/>
-    </row>
-    <row r="303" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D303" s="7"/>
-    </row>
-    <row r="304" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D304" s="7"/>
-    </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D305" s="7"/>
-    </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D306" s="7"/>
-    </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D307" s="7"/>
-    </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D308" s="7"/>
-    </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D309" s="7"/>
-    </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D310" s="7"/>
-    </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D311" s="7"/>
-    </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D312" s="7"/>
-    </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D313" s="7"/>
-    </row>
-    <row r="314" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D314" s="7"/>
-    </row>
-    <row r="315" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D315" s="7"/>
-    </row>
-    <row r="316" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D316" s="7"/>
-    </row>
-    <row r="317" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D317" s="7"/>
-    </row>
-    <row r="318" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D318" s="7"/>
-    </row>
-    <row r="319" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D319" s="7"/>
-    </row>
-    <row r="320" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D320" s="7"/>
-    </row>
-    <row r="321" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D321" s="7"/>
-    </row>
-    <row r="322" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D322" s="7"/>
-    </row>
-    <row r="323" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D323" s="7"/>
-    </row>
-    <row r="324" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D324" s="7"/>
-    </row>
-    <row r="325" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D325" s="7"/>
-    </row>
-    <row r="326" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D326" s="7"/>
-    </row>
-    <row r="327" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D327" s="7"/>
-    </row>
-    <row r="328" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D328" s="7"/>
-    </row>
-    <row r="329" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D329" s="7"/>
-    </row>
-    <row r="330" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D330" s="7"/>
-    </row>
-    <row r="331" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D331" s="7"/>
-    </row>
-    <row r="332" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D332" s="7"/>
-    </row>
-    <row r="333" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D333" s="7"/>
-    </row>
-    <row r="334" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D334" s="7"/>
-    </row>
-    <row r="335" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D335" s="7"/>
-    </row>
-    <row r="336" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D336" s="7"/>
-    </row>
-    <row r="337" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D337" s="8"/>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D191" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9:I186">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>